<commit_message>
Added changes to templates due to additions  RGB Color fill etc.  and stencil additions
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5ADE69-C7F1-404A-99C8-D6B880452462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21B9B16-6097-4326-A075-A0A07267AD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27435" yWindow="495" windowWidth="22200" windowHeight="14415" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="-24360" yWindow="420" windowWidth="24165" windowHeight="15300" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -187,21 +187,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{10638673-EC17-4823-B2FB-AD51FDAD3FB3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Select the fill color for the Stencil
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -212,7 +197,7 @@
     <author>Doug Vidakovich</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{ED9267BE-1A43-4825-9A17-5F51630FBD2D}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{646FA3E6-848A-4AC4-BB53-92B0D46FF81F}">
       <text>
         <r>
           <rPr>
@@ -235,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="203">
   <si>
     <t>mach_name</t>
   </si>
@@ -307,9 +292,6 @@
   </si>
   <si>
     <t>End</t>
-  </si>
-  <si>
-    <t>Light Blue</t>
   </si>
   <si>
     <t>Both</t>
@@ -334,9 +316,6 @@
     <t>Connect From</t>
   </si>
   <si>
-    <t>Fill Color</t>
-  </si>
-  <si>
     <t>Devices Count</t>
   </si>
   <si>
@@ -446,9 +425,6 @@
   </si>
   <si>
     <t>Colors</t>
-  </si>
-  <si>
-    <t>Light Green</t>
   </si>
   <si>
     <t>; Configuration</t>
@@ -802,6 +778,114 @@
   <si>
     <t>Stincel Label Font Size</t>
   </si>
+  <si>
+    <t>RGB Fill Color</t>
+  </si>
+  <si>
+    <t>Beige</t>
+  </si>
+  <si>
+    <t>Blue Alice</t>
+  </si>
+  <si>
+    <t>Blue Silver</t>
+  </si>
+  <si>
+    <t>Blue Steel</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Green Light</t>
+  </si>
+  <si>
+    <t>Green Lime</t>
+  </si>
+  <si>
+    <t>Green Sea</t>
+  </si>
+  <si>
+    <t>Khaki</t>
+  </si>
+  <si>
+    <t>Khaki Dark</t>
+  </si>
+  <si>
+    <t>Lime</t>
+  </si>
+  <si>
+    <t>Magenta</t>
+  </si>
+  <si>
+    <t>Mint</t>
+  </si>
+  <si>
+    <t>Navy</t>
+  </si>
+  <si>
+    <t>Olive</t>
+  </si>
+  <si>
+    <t>Olive Drab</t>
+  </si>
+  <si>
+    <t>Orange Light</t>
+  </si>
+  <si>
+    <t>Peach</t>
+  </si>
+  <si>
+    <t>Pink Light</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Tan</t>
+  </si>
+  <si>
+    <t>Teal</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>White Smoke</t>
+  </si>
+  <si>
+    <t>OC_Database</t>
+  </si>
+  <si>
+    <t>OC_Database2</t>
+  </si>
+  <si>
+    <t>OC_File</t>
+  </si>
+  <si>
+    <t>OC_File2</t>
+  </si>
+  <si>
+    <t>OC_Rectangle3R</t>
+  </si>
+  <si>
+    <t>OC_TableCell2</t>
+  </si>
+  <si>
+    <t>OC_SeeEmbedded</t>
+  </si>
+  <si>
+    <t>Fill Color</t>
+  </si>
 </sst>
 </file>
 
@@ -810,7 +894,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,6 +926,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -993,7 +1084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1076,7 +1167,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1113,10 +1203,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,6 +1233,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1455,11 +1553,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AG19"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,39 +1570,39 @@
     <col min="6" max="6" width="12.28515625" style="23" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="18" max="18" width="8" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" customWidth="1"/>
-    <col min="24" max="24" width="9.42578125" customWidth="1"/>
-    <col min="25" max="25" width="13.28515625" customWidth="1"/>
-    <col min="26" max="26" width="14.42578125" customWidth="1"/>
-    <col min="27" max="27" width="13.28515625" customWidth="1"/>
-    <col min="28" max="28" width="10.28515625" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" customWidth="1"/>
-    <col min="30" max="30" width="11" customWidth="1"/>
-    <col min="31" max="31" width="12" customWidth="1"/>
-    <col min="33" max="33" width="11.7109375" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="25" max="25" width="9.42578125" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" customWidth="1"/>
+    <col min="27" max="27" width="14.42578125" customWidth="1"/>
+    <col min="28" max="28" width="13.28515625" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" customWidth="1"/>
+    <col min="30" max="30" width="15.7109375" customWidth="1"/>
+    <col min="31" max="31" width="11" customWidth="1"/>
+    <col min="32" max="32" width="12" customWidth="1"/>
+    <col min="34" max="34" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>167</v>
+    <row r="1" spans="1:34" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1537,12 +1635,12 @@
         <v>9</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="40" t="s">
         <v>11</v>
       </c>
       <c r="U1" s="3" t="s">
@@ -1552,42 +1650,45 @@
         <v>13</v>
       </c>
       <c r="W1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA1" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB1" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC1" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y1" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z1" s="18" t="s">
+      <c r="AE1" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AF1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AG1" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="AC1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="AE1" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG1" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1611,8 +1712,8 @@
       <c r="U2" s="17"/>
       <c r="V2" s="17"/>
       <c r="W2" s="17"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="16"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="14"/>
       <c r="Z2" s="16"/>
       <c r="AA2" s="16"/>
       <c r="AB2" s="16"/>
@@ -1621,20 +1722,21 @@
       <c r="AE2" s="16"/>
       <c r="AF2" s="16"/>
       <c r="AG2" s="16"/>
-    </row>
-    <row r="3" spans="1:33" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="AH2" s="16"/>
+    </row>
+    <row r="3" spans="1:34" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="36" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>75</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -1662,32 +1764,33 @@
         <v>0</v>
       </c>
       <c r="W3" s="10"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="11"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="7"/>
       <c r="AA3" s="11"/>
-      <c r="AB3" s="7"/>
+      <c r="AB3" s="11"/>
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
-      <c r="AE3" s="11"/>
+      <c r="AE3" s="7"/>
       <c r="AF3" s="11"/>
-      <c r="AG3" s="7"/>
-    </row>
-    <row r="4" spans="1:33" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="36">
-        <v>0</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37" t="s">
-        <v>162</v>
-      </c>
-      <c r="F4" s="37"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="7"/>
+    </row>
+    <row r="4" spans="1:34" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="35">
+        <v>0</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="36"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -1713,32 +1816,33 @@
         <v>0</v>
       </c>
       <c r="W4" s="10"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="11"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="7"/>
       <c r="AA4" s="11"/>
-      <c r="AB4" s="7"/>
+      <c r="AB4" s="11"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
-      <c r="AE4" s="11"/>
+      <c r="AE4" s="7"/>
       <c r="AF4" s="11"/>
-      <c r="AG4" s="7"/>
-    </row>
-    <row r="5" spans="1:33" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" s="37"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="7"/>
+    </row>
+    <row r="5" spans="1:34" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="36"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -1764,32 +1868,33 @@
         <v>0</v>
       </c>
       <c r="W5" s="10"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="11"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="7"/>
       <c r="AA5" s="11"/>
-      <c r="AB5" s="7"/>
+      <c r="AB5" s="11"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
-      <c r="AE5" s="11"/>
+      <c r="AE5" s="7"/>
       <c r="AF5" s="11"/>
-      <c r="AG5" s="7"/>
-    </row>
-    <row r="6" spans="1:33" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="7"/>
+    </row>
+    <row r="6" spans="1:34" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46" t="s">
-        <v>160</v>
-      </c>
-      <c r="F6" s="46"/>
+      <c r="B6" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -1815,20 +1920,21 @@
         <v>0</v>
       </c>
       <c r="W6" s="10"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="11"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="7"/>
       <c r="AA6" s="11"/>
-      <c r="AB6" s="7"/>
+      <c r="AB6" s="11"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
-      <c r="AE6" s="11"/>
+      <c r="AE6" s="7"/>
       <c r="AF6" s="11"/>
-      <c r="AG6" s="7"/>
-    </row>
-    <row r="7" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="7"/>
+    </row>
+    <row r="7" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1852,8 +1958,8 @@
       <c r="U7" s="17"/>
       <c r="V7" s="17"/>
       <c r="W7" s="17"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="16"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="14"/>
       <c r="Z7" s="16"/>
       <c r="AA7" s="16"/>
       <c r="AB7" s="16"/>
@@ -1862,8 +1968,9 @@
       <c r="AE7" s="16"/>
       <c r="AF7" s="16"/>
       <c r="AG7" s="16"/>
-    </row>
-    <row r="8" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH7" s="16"/>
+    </row>
+    <row r="8" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>1</v>
       </c>
@@ -1871,10 +1978,10 @@
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
@@ -1903,18 +2010,19 @@
         <v>0</v>
       </c>
       <c r="W8" s="10"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="11"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="7"/>
       <c r="AA8" s="11"/>
-      <c r="AB8" s="7"/>
+      <c r="AB8" s="11"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
-      <c r="AE8" s="11"/>
+      <c r="AE8" s="7"/>
       <c r="AF8" s="11"/>
-      <c r="AG8" s="7"/>
-    </row>
-    <row r="9" spans="1:33" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="7"/>
+    </row>
+    <row r="9" spans="1:34" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>1</v>
       </c>
@@ -1922,13 +2030,13 @@
         <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="8"/>
@@ -1956,18 +2064,19 @@
         <v>0</v>
       </c>
       <c r="W9" s="10"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="11"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="7"/>
       <c r="AA9" s="11"/>
-      <c r="AB9" s="7"/>
+      <c r="AB9" s="11"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
-      <c r="AE9" s="11"/>
+      <c r="AE9" s="7"/>
       <c r="AF9" s="11"/>
-      <c r="AG9" s="7"/>
-    </row>
-    <row r="10" spans="1:33" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG9" s="11"/>
+      <c r="AH9" s="7"/>
+    </row>
+    <row r="10" spans="1:34" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1</v>
       </c>
@@ -1975,13 +2084,13 @@
         <v>14</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="8">
@@ -2010,21 +2119,22 @@
       <c r="V10" s="9">
         <v>1.125</v>
       </c>
-      <c r="W10" s="10"/>
+      <c r="W10" s="9"/>
       <c r="X10" s="8"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="11"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="7"/>
       <c r="AA10" s="11"/>
-      <c r="AB10" s="7"/>
+      <c r="AB10" s="11"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
-      <c r="AE10" s="11"/>
+      <c r="AE10" s="7"/>
       <c r="AF10" s="11"/>
-      <c r="AG10" s="7"/>
-    </row>
-    <row r="11" spans="1:33" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="7"/>
+    </row>
+    <row r="11" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -2048,8 +2158,8 @@
       <c r="U11" s="17"/>
       <c r="V11" s="17"/>
       <c r="W11" s="17"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="16"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="14"/>
       <c r="Z11" s="16"/>
       <c r="AA11" s="16"/>
       <c r="AB11" s="16"/>
@@ -2058,8 +2168,9 @@
       <c r="AE11" s="16"/>
       <c r="AF11" s="16"/>
       <c r="AG11" s="16"/>
-    </row>
-    <row r="12" spans="1:33" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="AH11" s="16"/>
+    </row>
+    <row r="12" spans="1:34" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>1</v>
       </c>
@@ -2067,13 +2178,13 @@
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -2086,7 +2197,7 @@
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
       <c r="P12" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q12" s="9"/>
       <c r="R12" s="7"/>
@@ -2102,29 +2213,28 @@
       <c r="V12" s="10">
         <v>0</v>
       </c>
-      <c r="W12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="11"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="7"/>
       <c r="AA12" s="11"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD12" s="7"/>
-      <c r="AE12" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE12" s="7"/>
       <c r="AF12" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AG12" s="7" t="s">
+      <c r="AH12" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>1</v>
       </c>
@@ -2132,16 +2242,16 @@
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -2153,7 +2263,7 @@
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q13" s="9"/>
       <c r="R13" s="7"/>
@@ -2169,29 +2279,28 @@
       <c r="V13" s="10">
         <v>0</v>
       </c>
-      <c r="W13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="11"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="7"/>
       <c r="AA13" s="11"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD13" s="7"/>
-      <c r="AE13" s="11" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE13" s="7"/>
       <c r="AF13" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="AG13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH13" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>1</v>
       </c>
@@ -2199,13 +2308,13 @@
         <v>14</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -2218,7 +2327,7 @@
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q14" s="9">
         <v>5001</v>
@@ -2237,18 +2346,19 @@
         <v>0</v>
       </c>
       <c r="W14" s="10"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="11"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="7"/>
       <c r="AA14" s="11"/>
-      <c r="AB14" s="7"/>
+      <c r="AB14" s="11"/>
       <c r="AC14" s="7"/>
       <c r="AD14" s="7"/>
-      <c r="AE14" s="11"/>
+      <c r="AE14" s="7"/>
       <c r="AF14" s="11"/>
-      <c r="AG14" s="7"/>
-    </row>
-    <row r="15" spans="1:33" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="7"/>
+    </row>
+    <row r="15" spans="1:34" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>1</v>
       </c>
@@ -2256,13 +2366,13 @@
         <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>104</v>
+        <v>111</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>101</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
@@ -2289,29 +2399,28 @@
       <c r="V15" s="10">
         <v>0</v>
       </c>
-      <c r="W15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="11"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="7"/>
       <c r="AA15" s="11"/>
-      <c r="AB15" s="7"/>
+      <c r="AB15" s="11"/>
       <c r="AC15" s="7"/>
       <c r="AD15" s="7"/>
-      <c r="AE15" s="11"/>
+      <c r="AE15" s="7"/>
       <c r="AF15" s="11"/>
-      <c r="AG15" s="7"/>
-    </row>
-    <row r="16" spans="1:33" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="7"/>
+    </row>
+    <row r="16" spans="1:34" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -2331,8 +2440,8 @@
       <c r="U16" s="17"/>
       <c r="V16" s="17"/>
       <c r="W16" s="17"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="16"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="14"/>
       <c r="Z16" s="16"/>
       <c r="AA16" s="16"/>
       <c r="AB16" s="16"/>
@@ -2341,8 +2450,9 @@
       <c r="AE16" s="16"/>
       <c r="AF16" s="16"/>
       <c r="AG16" s="16"/>
-    </row>
-    <row r="17" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH16" s="16"/>
+    </row>
+    <row r="17" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>2</v>
       </c>
@@ -2350,10 +2460,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
@@ -2382,18 +2492,19 @@
         <v>0</v>
       </c>
       <c r="W17" s="10"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="11"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="7"/>
       <c r="AA17" s="11"/>
-      <c r="AB17" s="7"/>
+      <c r="AB17" s="11"/>
       <c r="AC17" s="7"/>
       <c r="AD17" s="7"/>
-      <c r="AE17" s="11"/>
+      <c r="AE17" s="7"/>
       <c r="AF17" s="11"/>
-      <c r="AG17" s="7"/>
-    </row>
-    <row r="18" spans="1:33" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="7"/>
+    </row>
+    <row r="18" spans="1:34" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>2</v>
       </c>
@@ -2401,13 +2512,13 @@
         <v>14</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="8"/>
@@ -2435,18 +2546,19 @@
         <v>0</v>
       </c>
       <c r="W18" s="10"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="11"/>
+      <c r="X18" s="45"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="7"/>
       <c r="AA18" s="11"/>
-      <c r="AB18" s="7"/>
+      <c r="AB18" s="11"/>
       <c r="AC18" s="7"/>
       <c r="AD18" s="7"/>
-      <c r="AE18" s="11"/>
+      <c r="AE18" s="7"/>
       <c r="AF18" s="11"/>
-      <c r="AG18" s="7"/>
-    </row>
-    <row r="19" spans="1:33" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="7"/>
+    </row>
+    <row r="19" spans="1:34" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>2</v>
       </c>
@@ -2454,13 +2566,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="8">
@@ -2489,25 +2601,29 @@
       <c r="V19" s="9">
         <v>1.125</v>
       </c>
-      <c r="W19" s="10"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="11"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="7"/>
       <c r="AA19" s="11"/>
-      <c r="AB19" s="7"/>
+      <c r="AB19" s="11"/>
       <c r="AC19" s="7"/>
       <c r="AD19" s="7"/>
-      <c r="AE19" s="11"/>
+      <c r="AE19" s="7"/>
       <c r="AF19" s="11"/>
-      <c r="AG19" s="7"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="7"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X2:X18" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{1B1731AA-F2EB-4AE2-A6BB-599908765112}">
           <x14:formula1>
             <xm:f>Tables!$E$2:$E$16</xm:f>
@@ -2518,31 +2634,43 @@
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>X16:X19 AB2:AB5 AG2:AG5 W2:X5 X7:X11 AB7:AB19 AG7:AG19 W7:W19</xm:sqref>
+          <xm:sqref>Y16:Y19 Y7:Y11 Y2:Y5 X19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{03EA1083-D949-46E8-A92C-28C1E75A14F4}">
           <x14:formula1>
             <xm:f>Tables!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AE2:AE5 Z2:Z5 AE7:AE19 Z7:Z19</xm:sqref>
+          <xm:sqref>AF2:AF5 AA2:AA5 AF7:AF19 AA7:AA19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{296B0321-4EB3-4DBF-B3C7-556564F8D22F}">
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AA2:AA5 AF2:AF5 AA7:AA19 AF7:AF19</xm:sqref>
+          <xm:sqref>AB2:AB5 AG2:AG5 AB7:AB19 AG7:AG19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{D20E3002-F58D-4FAD-9CC5-854E38BB1BD9}">
           <x14:formula1>
             <xm:f>Tables!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2 F3:F19</xm:sqref>
+          <xm:sqref>F2:F19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{6CAB5953-26EB-4885-8C21-5C654465398A}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{144C7DAB-B2EC-4CB7-AB17-A3FF60790568}">
           <x14:formula1>
-            <xm:f>Tables!$M$2:$M$50</xm:f>
+            <xm:f>Tables!$K$2:$K$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D19</xm:sqref>
+          <xm:sqref>B2:B19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{72B07BB6-2E46-454E-98E1-28DF9333D6FA}">
+          <x14:formula1>
+            <xm:f>Tables!$N$2:$N$57</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{4D3802DC-9280-4A12-B1FF-B1C073FCAE84}">
+          <x14:formula1>
+            <xm:f>Tables!$A$2:$A$37</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2:W19 AC2:AC19 AH2:AH19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2568,7 +2696,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -2594,7 +2722,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
@@ -2602,16 +2730,16 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="D4" s="26" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2640,7 +2768,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="53" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="53"/>
       <c r="C10" s="53"/>
@@ -2655,37 +2783,37 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="F11" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="G11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="H11" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="I11" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="J11" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="K11" s="26" t="s">
         <v>58</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="26" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2738,7 +2866,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
@@ -2756,7 +2884,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="50"/>
@@ -2765,7 +2893,7 @@
       <c r="F16" s="50"/>
       <c r="G16" s="50"/>
       <c r="H16" s="56" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I16" s="56"/>
       <c r="J16" s="57"/>
@@ -2775,7 +2903,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
@@ -2823,20 +2951,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2875,10 +3003,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7C7130-C7ED-4E34-8ED2-CC717737ADA7}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2886,41 +3014,51 @@
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" style="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="M1" s="42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1"/>
+      <c r="I1" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1"/>
+      <c r="K1" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1" s="60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="C2" s="11"/>
       <c r="E2" s="11"/>
       <c r="G2" s="11"/>
       <c r="I2" s="11"/>
-      <c r="M2" s="43"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="11"/>
+      <c r="N2" s="42"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>15</v>
@@ -2929,38 +3067,46 @@
         <v>6</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M3" s="43" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="N3" s="42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="M4" s="43" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="N4" s="42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>23</v>
@@ -2969,328 +3115,431 @@
         <v>8</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="M5" s="43" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="N5" s="42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>44</v>
+        <v>169</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="M6" s="43" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="N6" s="42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>21</v>
+        <v>170</v>
       </c>
       <c r="E7" s="11">
         <v>9</v>
       </c>
-      <c r="M7" s="43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>24</v>
+        <v>171</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="43" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="N8" s="42" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>69</v>
+        <v>172</v>
       </c>
       <c r="E9" s="11">
         <v>10</v>
       </c>
-      <c r="M9" s="43" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="42" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="44" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="N10" s="43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="E11" s="11">
         <v>11</v>
       </c>
-      <c r="M11" s="43" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N11" s="42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M12" s="43" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+        <v>39</v>
+      </c>
+      <c r="N12" s="42" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="E13" s="11">
         <v>12</v>
       </c>
-      <c r="M13" s="43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="42" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="E14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M14" s="43" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="N14" s="42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>175</v>
+      </c>
       <c r="E15" s="11">
         <v>14</v>
       </c>
-      <c r="M15" s="43" t="s">
+      <c r="N15" s="42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="N17" s="42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="N18" s="42" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="N19" s="42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="N20" s="42" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="N21" s="42" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="N22" s="42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="N23" s="42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="N24" s="42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N25" s="42" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="N26" s="42" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="M16" s="44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M17" s="43" t="s">
+    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="N27" s="42" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M18" s="43" t="s">
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="N28" s="42" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M19" s="43" t="s">
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N29" s="43" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M20" s="43" t="s">
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30" s="42" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M21" s="43" t="s">
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="N31" s="42" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M22" s="43" t="s">
+    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="N32" s="43" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M23" s="43" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M24" s="43" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M25" s="43" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M26" s="43" t="s">
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="N33" s="42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="N34" s="42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="N35" s="42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="N36" s="42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N37" s="42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N38" s="42" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N39" s="42" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N40" s="42" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N41" s="42" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N42" s="42" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M27" s="43" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M28" s="43" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M29" s="44" t="s">
+    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N43" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N44" s="42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N45" s="42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N46" s="42" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M30" s="43" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M31" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M32" s="45" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M33" s="43" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M34" s="43" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M35" s="43" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="36" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M36" s="43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M37" s="43" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M38" s="43" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M39" s="43" t="s">
+    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N47" s="42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N48" s="42" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M40" s="43" t="s">
+    <row r="49" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N49" s="42" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M41" s="43" t="s">
+    <row r="50" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N50" s="61" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N51" s="42" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M42" s="43" t="s">
+    <row r="52" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N52" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N53" s="42" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M43" s="43" t="s">
+    <row r="54" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N54" s="42" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M44" s="43" t="s">
+    <row r="55" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N55" s="42" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="45" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M45" s="43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M46" s="43" t="s">
+    <row r="56" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N56" s="42" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M47" s="43" t="s">
+    <row r="57" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N57" s="42" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M48" s="43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M49" s="43" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="50" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M50" s="43" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="51" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M3:M45">
-    <sortCondition ref="M3:M45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M3:M57">
+    <sortCondition ref="M3:M57"/>
   </sortState>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:F2 N2:XFD2" xr:uid="{C5F5580C-CDE8-4810-9011-46F88A3A0968}">
-      <formula1>$A$4:$A$10</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
added some comments around the SaveDocument method
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21B9B16-6097-4326-A075-A0A07267AD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123F6BC0-6296-4E41-B9F5-F1505C6140FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24360" yWindow="420" windowWidth="24165" windowHeight="15300" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="-24675" yWindow="150" windowWidth="24165" windowHeight="15300" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="209">
   <si>
     <t>mach_name</t>
   </si>
@@ -785,15 +785,6 @@
     <t>Beige</t>
   </si>
   <si>
-    <t>Blue Alice</t>
-  </si>
-  <si>
-    <t>Blue Silver</t>
-  </si>
-  <si>
-    <t>Blue Steel</t>
-  </si>
-  <si>
     <t>Brown</t>
   </si>
   <si>
@@ -885,6 +876,33 @@
   </si>
   <si>
     <t>Fill Color</t>
+  </si>
+  <si>
+    <t>Blue Light</t>
+  </si>
+  <si>
+    <t>Blue Medium</t>
+  </si>
+  <si>
+    <t>Blue Bright</t>
+  </si>
+  <si>
+    <t>Gray Light</t>
+  </si>
+  <si>
+    <t>Gray Medium</t>
+  </si>
+  <si>
+    <t>Green LightMedium</t>
+  </si>
+  <si>
+    <t>Green Medium</t>
+  </si>
+  <si>
+    <t>Green Dark</t>
+  </si>
+  <si>
+    <t>Orange Medium</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1212,6 +1230,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1233,11 +1257,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1555,9 +1574,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,6 +1589,7 @@
     <col min="6" max="6" width="12.28515625" style="23" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="18" max="18" width="8" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" customWidth="1"/>
     <col min="24" max="24" width="13.42578125" customWidth="1"/>
     <col min="25" max="25" width="9.42578125" customWidth="1"/>
     <col min="26" max="26" width="13.28515625" customWidth="1"/>
@@ -1650,7 +1670,7 @@
         <v>13</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>167</v>
@@ -2213,7 +2233,9 @@
       <c r="V12" s="10">
         <v>0</v>
       </c>
-      <c r="W12" s="10"/>
+      <c r="W12" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="X12" s="10"/>
       <c r="Y12" s="8"/>
       <c r="Z12" s="7"/>
@@ -2279,7 +2301,9 @@
       <c r="V13" s="10">
         <v>0</v>
       </c>
-      <c r="W13" s="10"/>
+      <c r="W13" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="X13" s="10"/>
       <c r="Y13" s="8"/>
       <c r="Z13" s="7"/>
@@ -2399,7 +2423,9 @@
       <c r="V15" s="10">
         <v>0</v>
       </c>
-      <c r="W15" s="10"/>
+      <c r="W15" s="10" t="s">
+        <v>172</v>
+      </c>
       <c r="X15" s="46"/>
       <c r="Y15" s="8"/>
       <c r="Z15" s="7"/>
@@ -2668,7 +2694,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{4D3802DC-9280-4A12-B1FF-B1C073FCAE84}">
           <x14:formula1>
-            <xm:f>Tables!$A$2:$A$37</xm:f>
+            <xm:f>Tables!$A$2:$A$43</xm:f>
           </x14:formula1>
           <xm:sqref>W2:W19 AC2:AC19 AH2:AH19</xm:sqref>
         </x14:dataValidation>
@@ -2695,12 +2721,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
       <c r="E1" s="31"/>
       <c r="F1" s="31"/>
       <c r="G1" s="30"/>
@@ -2721,12 +2747,12 @@
       <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
@@ -2767,19 +2793,19 @@
       <c r="D8" s="13"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
@@ -2865,55 +2891,55 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="51"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="55"/>
       <c r="K15" s="27">
         <f>SUM(K12:K14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="56" t="s">
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="56"/>
-      <c r="J16" s="57"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="61"/>
       <c r="K16" s="28">
         <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="51"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="55"/>
       <c r="K17" s="26">
         <f>SUM(K15:K16)</f>
         <v>150</v>
@@ -2950,10 +2976,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="63"/>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3005,19 +3031,19 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="62" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" style="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -3043,7 +3069,7 @@
       </c>
       <c r="L1"/>
       <c r="M1"/>
-      <c r="N1" s="60" t="s">
+      <c r="N1" s="47" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3127,7 +3153,7 @@
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>24</v>
@@ -3148,7 +3174,7 @@
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="E7" s="11">
         <v>9</v>
@@ -3159,7 +3185,7 @@
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>37</v>
@@ -3170,7 +3196,7 @@
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E9" s="11">
         <v>10</v>
@@ -3192,7 +3218,7 @@
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E11" s="11">
         <v>11</v>
@@ -3209,23 +3235,23 @@
         <v>39</v>
       </c>
       <c r="N12" s="42" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>21</v>
+        <v>203</v>
       </c>
       <c r="E13" s="11">
         <v>12</v>
       </c>
       <c r="N13" s="42" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>174</v>
+      <c r="A14" s="50" t="s">
+        <v>204</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>40</v>
@@ -3236,7 +3262,7 @@
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="E15" s="11">
         <v>14</v>
@@ -3247,7 +3273,7 @@
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>41</v>
@@ -3258,7 +3284,7 @@
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="N17" s="42" t="s">
         <v>135</v>
@@ -3266,7 +3292,7 @@
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="N18" s="42" t="s">
         <v>136</v>
@@ -3274,7 +3300,7 @@
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="N19" s="42" t="s">
         <v>137</v>
@@ -3282,23 +3308,23 @@
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="N20" s="42" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="N21" s="42" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="N22" s="42" t="s">
         <v>125</v>
@@ -3306,7 +3332,7 @@
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="N23" s="42" t="s">
         <v>110</v>
@@ -3314,7 +3340,7 @@
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="N24" s="42" t="s">
         <v>126</v>
@@ -3322,7 +3348,7 @@
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="N25" s="42" t="s">
         <v>127</v>
@@ -3330,7 +3356,7 @@
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="N26" s="42" t="s">
         <v>128</v>
@@ -3338,7 +3364,7 @@
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="N27" s="42" t="s">
         <v>129</v>
@@ -3346,7 +3372,7 @@
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N28" s="42" t="s">
         <v>130</v>
@@ -3354,7 +3380,7 @@
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="N29" s="43" t="s">
         <v>131</v>
@@ -3362,7 +3388,7 @@
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="N30" s="42" t="s">
         <v>132</v>
@@ -3370,15 +3396,15 @@
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="N31" s="42" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>190</v>
+      <c r="A32" s="50" t="s">
+        <v>208</v>
       </c>
       <c r="N32" s="43" t="s">
         <v>134</v>
@@ -3386,7 +3412,7 @@
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="N33" s="42" t="s">
         <v>108</v>
@@ -3394,7 +3420,7 @@
     </row>
     <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="N34" s="42" t="s">
         <v>112</v>
@@ -3402,7 +3428,7 @@
     </row>
     <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="N35" s="42" t="s">
         <v>141</v>
@@ -3410,7 +3436,7 @@
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>194</v>
+        <v>25</v>
       </c>
       <c r="N36" s="42" t="s">
         <v>142</v>
@@ -3418,38 +3444,56 @@
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>26</v>
+        <v>186</v>
       </c>
       <c r="N37" s="42" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>187</v>
+      </c>
       <c r="N38" s="42" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>188</v>
+      </c>
       <c r="N39" s="42" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>189</v>
+      </c>
       <c r="N40" s="42" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>190</v>
+      </c>
       <c r="N41" s="42" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="N42" s="42" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="N43" s="42" t="s">
         <v>143</v>
       </c>
@@ -3485,8 +3529,8 @@
       </c>
     </row>
     <row r="50" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N50" s="61" t="s">
-        <v>200</v>
+      <c r="N50" s="48" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated the Json file to the lastest values.
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11ACA9BD-7875-45C2-AC12-3FB9E43A11D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181BB8D-6614-43C8-8E8D-3FE3212513CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27435" yWindow="270" windowWidth="26550" windowHeight="14445" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
@@ -322,9 +322,6 @@
     <t>Connect To</t>
   </si>
   <si>
-    <t>ShapeLabel FontSize</t>
-  </si>
-  <si>
     <t>Shape Type</t>
   </si>
   <si>
@@ -933,6 +930,9 @@
   </si>
   <si>
     <t>6 pt</t>
+  </si>
+  <si>
+    <t>Shape Label Font Size</t>
   </si>
 </sst>
 </file>
@@ -1606,8 +1606,8 @@
   <dimension ref="A1:AJ19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,25 +1635,25 @@
   <sheetData>
     <row r="1" spans="1:36" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1701,51 +1701,51 @@
         <v>13</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="Z1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AB1" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AC1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="AC1" s="18" t="s">
-        <v>76</v>
-      </c>
       <c r="AD1" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE1" s="5" t="s">
         <v>31</v>
       </c>
       <c r="AF1" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG1" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="AI1" s="19" t="s">
-        <v>80</v>
-      </c>
       <c r="AJ1" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1785,17 +1785,17 @@
     </row>
     <row r="3" spans="1:36" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -1842,14 +1842,14 @@
         <v>0</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F4" s="36"/>
       <c r="G4" s="8"/>
@@ -1893,17 +1893,17 @@
     </row>
     <row r="5" spans="1:36" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="36" t="s">
         <v>103</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>104</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="36"/>
       <c r="G5" s="8"/>
@@ -1950,14 +1950,14 @@
         <v>0</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" s="8"/>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="7" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -2047,10 +2047,10 @@
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
@@ -2101,10 +2101,10 @@
         <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>27</v>
@@ -2157,10 +2157,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>28</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="11" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -2255,13 +2255,13 @@
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -2274,7 +2274,7 @@
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
       <c r="P12" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q12" s="9"/>
       <c r="R12" s="7"/>
@@ -2301,11 +2301,11 @@
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
       <c r="AE12" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AF12" s="7"/>
       <c r="AG12" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AH12" s="11" t="s">
         <v>15</v>
@@ -2314,7 +2314,7 @@
         <v>18</v>
       </c>
       <c r="AJ12" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:36" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2325,16 +2325,16 @@
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -2346,7 +2346,7 @@
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q13" s="9"/>
       <c r="R13" s="7"/>
@@ -2373,17 +2373,17 @@
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
       <c r="AE13" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AF13" s="7"/>
       <c r="AG13" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH13" s="11" t="s">
         <v>24</v>
       </c>
       <c r="AI13" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AJ13" s="7"/>
     </row>
@@ -2395,13 +2395,13 @@
         <v>14</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -2414,7 +2414,7 @@
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q14" s="9">
         <v>5001</v>
@@ -2455,13 +2455,13 @@
         <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
@@ -2489,11 +2489,11 @@
         <v>0</v>
       </c>
       <c r="W15" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X15" s="46"/>
       <c r="Y15" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z15" s="7"/>
       <c r="AA15" s="11"/>
@@ -2504,7 +2504,7 @@
         <v>21</v>
       </c>
       <c r="AD15" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE15" s="7"/>
       <c r="AF15" s="7"/>
@@ -2515,13 +2515,13 @@
     </row>
     <row r="16" spans="1:36" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -2563,10 +2563,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
@@ -2617,10 +2617,10 @@
         <v>14</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>27</v>
@@ -2673,10 +2673,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>28</v>
@@ -2811,7 +2811,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="57"/>
       <c r="C3" s="57"/>
@@ -2845,16 +2845,16 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C4" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="D4" s="26" t="s">
         <v>48</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2883,7 +2883,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="58"/>
       <c r="C10" s="58"/>
@@ -2898,37 +2898,37 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>47</v>
-      </c>
       <c r="C11" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="E11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="F11" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="G11" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="H11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="I11" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="J11" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="K11" s="26" t="s">
         <v>57</v>
-      </c>
-      <c r="K11" s="26" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2981,7 +2981,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="55"/>
       <c r="C15" s="55"/>
@@ -2999,7 +2999,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="55"/>
       <c r="C16" s="55"/>
@@ -3008,7 +3008,7 @@
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
       <c r="H16" s="61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I16" s="61"/>
       <c r="J16" s="62"/>
@@ -3018,7 +3018,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="55"/>
       <c r="C17" s="55"/>
@@ -3066,20 +3066,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="C2" s="26" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3121,15 +3121,15 @@
   <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" customWidth="1"/>
@@ -3138,32 +3138,32 @@
   <sheetData>
     <row r="1" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>32</v>
+        <v>218</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H1"/>
       <c r="I1" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J1"/>
       <c r="K1" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L1"/>
       <c r="M1" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N1"/>
       <c r="O1" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3178,7 +3178,7 @@
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>15</v>
@@ -3187,20 +3187,20 @@
         <v>6</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O3" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3211,23 +3211,23 @@
         <v>20</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O4" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3241,80 +3241,80 @@
         <v>8</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O5" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O6" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E7" s="11">
         <v>9</v>
       </c>
       <c r="M7" s="51" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M8" s="51" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O8" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E9" s="11">
         <v>10</v>
       </c>
       <c r="O9" s="42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3322,54 +3322,54 @@
         <v>22</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O10" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E11" s="11">
         <v>11</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O12" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E13" s="11">
         <v>12</v>
       </c>
       <c r="O13" s="42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O14" s="42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3380,122 +3380,122 @@
         <v>14</v>
       </c>
       <c r="O15" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O16" s="43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O17" s="42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O18" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O19" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O20" s="42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O21" s="42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O22" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O23" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O24" s="42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O25" s="42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O26" s="42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O27" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O28" s="42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O29" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3503,47 +3503,47 @@
         <v>18</v>
       </c>
       <c r="O30" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O31" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O32" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O33" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O34" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O35" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3551,55 +3551,55 @@
         <v>25</v>
       </c>
       <c r="O36" s="42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O37" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O38" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O39" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O40" s="42" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O41" s="42" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O42" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3607,77 +3607,77 @@
         <v>26</v>
       </c>
       <c r="O43" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O44" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O45" s="42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O46" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O47" s="42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O48" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O49" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O50" s="48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O51" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O52" s="42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O53" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O54" s="42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O55" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O56" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O57" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed the OC_DashOutline color issue.  this is a transparent type stencil.  Only the LineColor will be colored no fill. updated the user guide updated the Excel templates Updated the Visio Stencil (all stencils are Top-Left position)
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181BB8D-6614-43C8-8E8D-3FE3212513CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E9A888-1D5B-44D8-8283-C9C880D47180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27435" yWindow="270" windowWidth="26550" windowHeight="14445" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="-27510" yWindow="285" windowWidth="26550" windowHeight="14445" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="218">
   <si>
     <t>mach_name</t>
   </si>
@@ -915,9 +915,6 @@
   </si>
   <si>
     <t>2.25 pt</t>
-  </si>
-  <si>
-    <t>6.0 pt</t>
   </si>
   <si>
     <t>2 pt</t>
@@ -1606,8 +1603,8 @@
   <dimension ref="A1:AJ19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,7 +2146,7 @@
       <c r="AI9" s="7"/>
       <c r="AJ9" s="7"/>
     </row>
-    <row r="10" spans="1:36" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" s="12" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1</v>
       </c>
@@ -2166,8 +2163,8 @@
         <v>28</v>
       </c>
       <c r="F10" s="21"/>
-      <c r="G10" s="8">
-        <v>10</v>
+      <c r="G10" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -2314,7 +2311,7 @@
         <v>18</v>
       </c>
       <c r="AJ12" s="7" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:36" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2504,7 +2501,7 @@
         <v>21</v>
       </c>
       <c r="AD15" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AE15" s="7"/>
       <c r="AF15" s="7"/>
@@ -2665,7 +2662,7 @@
       <c r="AI18" s="7"/>
       <c r="AJ18" s="7"/>
     </row>
-    <row r="19" spans="1:36" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>2</v>
       </c>
@@ -3120,20 +3117,20 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" style="49" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -3144,7 +3141,7 @@
         <v>16</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>80</v>
@@ -3224,7 +3221,7 @@
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O4" s="42" t="s">
         <v>113</v>
@@ -3272,7 +3269,7 @@
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O6" s="42" t="s">
         <v>115</v>
@@ -3286,7 +3283,7 @@
         <v>9</v>
       </c>
       <c r="M7" s="51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O7" s="42" t="s">
         <v>116</v>
@@ -3300,7 +3297,7 @@
         <v>36</v>
       </c>
       <c r="M8" s="51" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O8" s="42" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
changed .Equal to .IndexOf
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E9A888-1D5B-44D8-8283-C9C880D47180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FBEE2C-7FA9-4E74-899E-4CA35E890F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27510" yWindow="285" windowWidth="26550" windowHeight="14445" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="-28710" yWindow="75" windowWidth="28830" windowHeight="15780" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="222">
   <si>
     <t>mach_name</t>
   </si>
@@ -930,6 +930,18 @@
   </si>
   <si>
     <t>Shape Label Font Size</t>
+  </si>
+  <si>
+    <t>Server:21</t>
+  </si>
+  <si>
+    <t>Server:22</t>
+  </si>
+  <si>
+    <t>OISInterfaces:23</t>
+  </si>
+  <si>
+    <t>OC_Server:24</t>
   </si>
 </sst>
 </file>
@@ -1600,11 +1612,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AJ19"/>
+  <dimension ref="A1:AJ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2720,9 +2732,321 @@
       <c r="AI19" s="7"/>
       <c r="AJ19" s="7"/>
     </row>
+    <row r="20" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="16"/>
+      <c r="AB20" s="16"/>
+      <c r="AC20" s="16"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="16"/>
+      <c r="AF20" s="16"/>
+      <c r="AG20" s="16"/>
+      <c r="AH20" s="16"/>
+      <c r="AI20" s="16"/>
+      <c r="AJ20" s="16"/>
+    </row>
+    <row r="21" spans="1:36" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>2</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="10">
+        <v>4.875</v>
+      </c>
+      <c r="T21" s="10">
+        <v>6.25</v>
+      </c>
+      <c r="U21" s="10">
+        <v>0</v>
+      </c>
+      <c r="V21" s="10">
+        <v>0</v>
+      </c>
+      <c r="W21" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="7"/>
+      <c r="AE21" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ21" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>2</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="10">
+        <v>6.125</v>
+      </c>
+      <c r="T22" s="10">
+        <v>5.7969999999999997</v>
+      </c>
+      <c r="U22" s="10">
+        <v>0</v>
+      </c>
+      <c r="V22" s="10">
+        <v>0</v>
+      </c>
+      <c r="W22" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="7"/>
+      <c r="AE22" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF22" s="7"/>
+      <c r="AG22" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI22" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ22" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>2</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q23" s="9">
+        <v>5001</v>
+      </c>
+      <c r="R23" s="7"/>
+      <c r="S23" s="10">
+        <v>7.5</v>
+      </c>
+      <c r="T23" s="10">
+        <v>6.0750000000000002</v>
+      </c>
+      <c r="U23" s="10">
+        <v>0</v>
+      </c>
+      <c r="V23" s="10">
+        <v>0</v>
+      </c>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="11"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7"/>
+    </row>
+    <row r="24" spans="1:36" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>2</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="10">
+        <v>4.8959999999999999</v>
+      </c>
+      <c r="T24" s="10">
+        <v>4.75</v>
+      </c>
+      <c r="U24" s="10">
+        <v>0</v>
+      </c>
+      <c r="V24" s="10">
+        <v>0</v>
+      </c>
+      <c r="W24" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="X24" s="46"/>
+      <c r="Y24" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD24" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE24" s="7"/>
+      <c r="AF24" s="7"/>
+      <c r="AG24" s="11"/>
+      <c r="AH24" s="11"/>
+      <c r="AI24" s="7"/>
+      <c r="AJ24" s="7"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X2:X18" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X2:X18 X20:X24" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2734,55 +3058,55 @@
           <x14:formula1>
             <xm:f>Tables!$E$2:$E$16</xm:f>
           </x14:formula1>
-          <xm:sqref>G8:G11 G16:G19</xm:sqref>
+          <xm:sqref>G8:G11 G16:G24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{E07EFBB9-D469-4A17-B52C-CFA259DBA49F}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>Y16:Y19 Y7:Y11 Y2:Y5 X19</xm:sqref>
+          <xm:sqref>X19 Y7:Y11 Y2:Y5 Y16:Y20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{03EA1083-D949-46E8-A92C-28C1E75A14F4}">
           <x14:formula1>
             <xm:f>Tables!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AG2:AG5 AA2:AA5 AG7:AG19 AA7:AA19</xm:sqref>
+          <xm:sqref>AG2:AG5 AA2:AA5 AA7:AA24 AG7:AG24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{296B0321-4EB3-4DBF-B3C7-556564F8D22F}">
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AB2:AB5 AH2:AH5 AB7:AB19 AH7:AH19</xm:sqref>
+          <xm:sqref>AB2:AB5 AH2:AH5 AH7:AH24 AB7:AB24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{D20E3002-F58D-4FAD-9CC5-854E38BB1BD9}">
           <x14:formula1>
             <xm:f>Tables!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F19</xm:sqref>
+          <xm:sqref>F2:F24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{144C7DAB-B2EC-4CB7-AB17-A3FF60790568}">
           <x14:formula1>
             <xm:f>Tables!$K$2:$K$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B19</xm:sqref>
+          <xm:sqref>B2:B24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{72B07BB6-2E46-454E-98E1-28DF9333D6FA}">
           <x14:formula1>
             <xm:f>Tables!$O$2:$O$57</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D19</xm:sqref>
+          <xm:sqref>D2:D24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{4D3802DC-9280-4A12-B1FF-B1C073FCAE84}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>W2:W19 AI2:AI19 AC2:AC19</xm:sqref>
+          <xm:sqref>AI2:AI24 AC2:AC24 W2:W24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{1FC98D1B-D5FE-4286-BF65-FB36E506A4BC}">
           <x14:formula1>
             <xm:f>Tables!$M$2:$M$8</xm:f>
           </x14:formula1>
-          <xm:sqref>AD2:AD19 AJ2:AJ19</xm:sqref>
+          <xm:sqref>AJ2:AJ24 AD2:AD24</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated the excel templates
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FBEE2C-7FA9-4E74-899E-4CA35E890F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB64C53-7B41-4FC5-B1FE-A177740971AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28710" yWindow="75" windowWidth="28830" windowHeight="15780" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="1785" yWindow="2040" windowWidth="27225" windowHeight="14730" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="219">
   <si>
     <t>mach_name</t>
   </si>
@@ -657,12 +657,6 @@
     <t>OC_Group2</t>
   </si>
   <si>
-    <t>OC_Group3</t>
-  </si>
-  <si>
-    <t>OC_Group4</t>
-  </si>
-  <si>
     <t>OC_IconKey</t>
   </si>
   <si>
@@ -681,12 +675,6 @@
     <t>OC_Ethernet</t>
   </si>
   <si>
-    <t>OC_Ethernet2</t>
-  </si>
-  <si>
-    <t>OC_Ethernet3</t>
-  </si>
-  <si>
     <t>OC_Process</t>
   </si>
   <si>
@@ -712,9 +700,6 @@
   </si>
   <si>
     <t>OC_Supply</t>
-  </si>
-  <si>
-    <t>OC_TabelCell</t>
   </si>
   <si>
     <t>OC_TagLabeler</t>
@@ -942,6 +927,12 @@
   </si>
   <si>
     <t>OC_Server:24</t>
+  </si>
+  <si>
+    <t>OC_Ethernet2H</t>
+  </si>
+  <si>
+    <t>OC_TableCell</t>
   </si>
 </sst>
 </file>
@@ -1614,9 +1605,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA24" sqref="AA24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,16 +1644,16 @@
         <v>106</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1710,10 +1701,10 @@
         <v>13</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>29</v>
@@ -1731,7 +1722,7 @@
         <v>75</v>
       </c>
       <c r="AD1" s="18" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AE1" s="5" t="s">
         <v>31</v>
@@ -1749,7 +1740,7 @@
         <v>79</v>
       </c>
       <c r="AJ1" s="19" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1804,7 +1795,7 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -1858,7 +1849,7 @@
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F4" s="36"/>
       <c r="G4" s="8"/>
@@ -1962,11 +1953,11 @@
         <v>102</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" s="8"/>
@@ -2323,7 +2314,7 @@
         <v>18</v>
       </c>
       <c r="AJ12" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:36" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2343,7 +2334,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -2392,7 +2383,7 @@
         <v>24</v>
       </c>
       <c r="AI13" s="7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="AJ13" s="7"/>
     </row>
@@ -2464,7 +2455,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>110</v>
@@ -2472,7 +2463,9 @@
       <c r="E15" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -2498,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="W15" s="10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="X15" s="46"/>
       <c r="Y15" s="8" t="s">
@@ -2513,7 +2506,7 @@
         <v>21</v>
       </c>
       <c r="AD15" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AE15" s="7"/>
       <c r="AF15" s="7"/>
@@ -2741,7 +2734,7 @@
       <c r="D20" s="14"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="8"/>
+      <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -2780,7 +2773,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>110</v>
@@ -2816,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="W21" s="10" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="X21" s="10"/>
       <c r="Y21" s="8"/>
@@ -2826,7 +2819,7 @@
       <c r="AC21" s="7"/>
       <c r="AD21" s="7"/>
       <c r="AE21" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="AF21" s="7"/>
       <c r="AG21" s="11" t="s">
@@ -2839,7 +2832,7 @@
         <v>17</v>
       </c>
       <c r="AJ21" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:36" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2850,7 +2843,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>110</v>
@@ -2859,7 +2852,7 @@
         <v>88</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -2888,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="W22" s="10" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="X22" s="10"/>
       <c r="Y22" s="8"/>
@@ -2898,7 +2891,7 @@
       <c r="AC22" s="7"/>
       <c r="AD22" s="7"/>
       <c r="AE22" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="AF22" s="7"/>
       <c r="AG22" s="11" t="s">
@@ -2908,10 +2901,10 @@
         <v>24</v>
       </c>
       <c r="AI22" s="7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="AJ22" s="7" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:36" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2922,7 +2915,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>111</v>
@@ -2982,7 +2975,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>110</v>
@@ -2991,7 +2984,7 @@
         <v>100</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>37</v>
@@ -3020,11 +3013,11 @@
         <v>0</v>
       </c>
       <c r="W24" s="10" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="X24" s="46"/>
       <c r="Y24" s="8" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="Z24" s="7"/>
       <c r="AA24" s="11"/>
@@ -3035,7 +3028,7 @@
         <v>25</v>
       </c>
       <c r="AD24" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AE24" s="7"/>
       <c r="AF24" s="7"/>
@@ -3090,12 +3083,6 @@
           </x14:formula1>
           <xm:sqref>B2:B24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{72B07BB6-2E46-454E-98E1-28DF9333D6FA}">
-          <x14:formula1>
-            <xm:f>Tables!$O$2:$O$57</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D24</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{4D3802DC-9280-4A12-B1FF-B1C073FCAE84}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$43</xm:f>
@@ -3107,6 +3094,12 @@
             <xm:f>Tables!$M$2:$M$8</xm:f>
           </x14:formula1>
           <xm:sqref>AJ2:AJ24 AD2:AD24</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{72B07BB6-2E46-454E-98E1-28DF9333D6FA}">
+          <x14:formula1>
+            <xm:f>Tables!$O$2:$O$54</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D24</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3439,10 +3432,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7C7130-C7ED-4E34-8ED2-CC717737ADA7}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:O69"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E16"/>
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,14 +3458,14 @@
         <v>16</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>80</v>
       </c>
       <c r="H1"/>
       <c r="I1" s="41" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J1"/>
       <c r="K1" s="33" t="s">
@@ -3480,7 +3473,7 @@
       </c>
       <c r="L1"/>
       <c r="M1" s="33" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="N1"/>
       <c r="O1" s="47" t="s">
@@ -3499,7 +3492,7 @@
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>15</v>
@@ -3511,14 +3504,14 @@
         <v>81</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>67</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="13" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O3" s="42" t="s">
         <v>112</v>
@@ -3538,14 +3531,14 @@
         <v>82</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>69</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="13" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="O4" s="42" t="s">
         <v>113</v>
@@ -3569,7 +3562,7 @@
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="O5" s="42" t="s">
         <v>114</v>
@@ -3577,7 +3570,7 @@
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>24</v>
@@ -3593,7 +3586,7 @@
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="13" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O6" s="42" t="s">
         <v>115</v>
@@ -3601,13 +3594,13 @@
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E7" s="11">
         <v>9</v>
       </c>
       <c r="M7" s="51" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="O7" s="42" t="s">
         <v>116</v>
@@ -3615,13 +3608,13 @@
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>36</v>
       </c>
       <c r="M8" s="51" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="O8" s="42" t="s">
         <v>117</v>
@@ -3629,7 +3622,7 @@
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E9" s="11">
         <v>10</v>
@@ -3651,7 +3644,7 @@
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E11" s="11">
         <v>11</v>
@@ -3668,23 +3661,23 @@
         <v>38</v>
       </c>
       <c r="O12" s="42" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E13" s="11">
         <v>12</v>
       </c>
       <c r="O13" s="42" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="50" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>39</v>
@@ -3706,7 +3699,7 @@
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>40</v>
@@ -3717,106 +3710,106 @@
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O17" s="42" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="O18" s="42" t="s">
-        <v>135</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="O19" s="42" t="s">
-        <v>136</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="O20" s="42" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="O21" s="42" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="O22" s="42" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="O23" s="42" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="O24" s="42" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="O25" s="42" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="O26" s="42" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="O27" s="42" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="O28" s="42" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="O29" s="43" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3824,47 +3817,47 @@
         <v>18</v>
       </c>
       <c r="O30" s="42" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="O31" s="42" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="O32" s="43" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="O33" s="42" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="O34" s="42" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="O35" s="42" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3872,55 +3865,55 @@
         <v>25</v>
       </c>
       <c r="O36" s="42" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="O37" s="42" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="O38" s="42" t="s">
-        <v>138</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="O39" s="42" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="O40" s="42" t="s">
-        <v>195</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="O41" s="42" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="O42" s="42" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3928,79 +3921,67 @@
         <v>26</v>
       </c>
       <c r="O43" s="42" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O44" s="42" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O45" s="42" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O46" s="42" t="s">
-        <v>139</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O47" s="42" t="s">
-        <v>154</v>
+      <c r="O47" s="48" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O48" s="42" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O49" s="42" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O50" s="48" t="s">
-        <v>196</v>
+      <c r="O50" s="42" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O51" s="42" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O52" s="42" t="s">
-        <v>108</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O53" s="42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O54" s="42" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="55" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O55" s="42" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="56" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O56" s="42" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="57" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O57" s="42" t="s">
-        <v>152</v>
-      </c>
-    </row>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4010,12 +3991,9 @@
     <row r="64" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:N57">
-    <sortCondition ref="N3:N57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:N54">
+    <sortCondition ref="N3:N54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the creation of the exceldata folder is it does not exist adjusted the template files
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A4CC9A-A7D0-4E28-B4DB-391001D514D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2861D9A5-A743-4503-91C4-B17AF93E7928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27765" yWindow="405" windowWidth="27210" windowHeight="14730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23895" yWindow="330" windowWidth="23535" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -1678,9 +1678,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,58 +1970,58 @@
       <c r="AJ4" s="11"/>
     </row>
     <row r="5" spans="1:36" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="12">
-        <v>0</v>
-      </c>
-      <c r="T5" s="12">
-        <v>0</v>
-      </c>
-      <c r="U5" s="12">
-        <v>0</v>
-      </c>
-      <c r="V5" s="12">
-        <v>0</v>
-      </c>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="11"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="16">
+        <v>0</v>
+      </c>
+      <c r="T5" s="16">
+        <v>0</v>
+      </c>
+      <c r="U5" s="16">
+        <v>0</v>
+      </c>
+      <c r="V5" s="16">
+        <v>0</v>
+      </c>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="14"/>
     </row>
     <row r="6" spans="1:36" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
@@ -4427,7 +4427,7 @@
       <c r="AI48" s="14"/>
       <c r="AJ48" s="14"/>
     </row>
-    <row r="49" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>1</v>
       </c>

</xml_diff>